<commit_message>
Leetcode - March05 2021 and DailyByte problems(all catchup for last one week)
</commit_message>
<xml_diff>
--- a/src/questions/questions-by-company.xlsx
+++ b/src/questions/questions-by-company.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RER\IdeaProjects\problem_practise\src\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFD9F05-492E-4329-A72D-0FE7F3B6CFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B62BC26-CBF9-49A6-BD53-ACE5CC210F85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="-120" windowWidth="27720" windowHeight="16440" xr2:uid="{E4F0F56F-AAA1-44A3-9F59-A06C3D251C3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4178" uniqueCount="817">
   <si>
     <t>ID</t>
   </si>
@@ -2455,6 +2455,36 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>aci</t>
+  </si>
+  <si>
+    <t>mamm</t>
+  </si>
+  <si>
+    <t>acmI</t>
+  </si>
+  <si>
+    <t>dose</t>
+  </si>
+  <si>
+    <t>aclr</t>
+  </si>
+  <si>
+    <t>acearch t</t>
+  </si>
+  <si>
+    <t>doumbersr</t>
+  </si>
+  <si>
+    <t>acumbersI</t>
+  </si>
+  <si>
+    <t>maoI</t>
+  </si>
+  <si>
+    <t>acr</t>
   </si>
 </sst>
 </file>
@@ -2506,13 +2536,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -2832,8 +2865,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E692"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="E179" sqref="E179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,7 +3446,7 @@
       <c r="A40" s="3">
         <v>438</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -5327,11 +5360,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>1</v>
       </c>
-      <c r="B177" s="3" t="s">
+      <c r="B177" s="4" t="s">
         <v>232</v>
       </c>
       <c r="C177" s="3" t="s">
@@ -5341,7 +5374,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>167</v>
       </c>
@@ -5354,8 +5387,11 @@
       <c r="D178" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E178" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>170</v>
       </c>
@@ -5369,7 +5405,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>653</v>
       </c>
@@ -5383,7 +5419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>263</v>
       </c>
@@ -5397,7 +5433,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>929</v>
       </c>
@@ -5411,7 +5447,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>804</v>
       </c>
@@ -5425,7 +5461,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>242</v>
       </c>
@@ -5439,7 +5475,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>941</v>
       </c>
@@ -5453,7 +5489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>125</v>
       </c>
@@ -5467,7 +5503,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>680</v>
       </c>
@@ -5481,7 +5517,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>20</v>
       </c>
@@ -5495,7 +5531,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>193</v>
       </c>
@@ -5509,7 +5545,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>953</v>
       </c>
@@ -5523,7 +5559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>290</v>
       </c>
@@ -5537,7 +5573,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>914</v>
       </c>

</xml_diff>